<commit_message>
updated keywords, website url
</commit_message>
<xml_diff>
--- a/keywords_ofb_india.xlsx
+++ b/keywords_ofb_india.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24430"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://morningstaronline-my.sharepoint.com/personal/tiberiu_pintilie_morningstar_com/Documents/projects/cwr/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{54A8349F-C593-4A47-8AB1-4B7B78D2BDF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BC4CAB7C-B8C2-446E-9673-C3B4378D8DBE}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="8_{54A8349F-C593-4A47-8AB1-4B7B78D2BDF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A74880FB-1828-4270-A2D4-DAF34099AABB}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="19">
   <si>
     <t>apers</t>
   </si>
@@ -79,6 +79,9 @@
   </si>
   <si>
     <t>Indicator</t>
+  </si>
+  <si>
+    <t>submunition</t>
   </si>
 </sst>
 </file>
@@ -408,7 +411,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B24"/>
+  <dimension ref="A1:B25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
@@ -508,7 +511,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>5</v>
       </c>
@@ -516,36 +519,45 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
-        <v>8</v>
+    <row r="13" spans="1:2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="1" t="s">
+        <v>5</v>
       </c>
       <c r="B13" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>8</v>
       </c>
       <c r="B14" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>8</v>
+      </c>
+      <c r="B15" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A20" s="1"/>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:1" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="21" spans="1:1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A21" s="1"/>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A22" s="1"/>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A23" s="1"/>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A24" s="1"/>
+    </row>
+    <row r="25" spans="1:1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>